<commit_message>
added dates to epoch
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/scheduling/data/2023EarthAssets.xlsx
+++ b/Assets/StreamingAssets/scheduling/data/2023EarthAssets.xlsx
@@ -706,12 +706,12 @@
   <autoFilter ref="A2:AT1130">
     <filterColumn colId="0">
       <filters>
-        <filter val="Facility"/>
+        <filter val="Satellite"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A3:AT1132">
-    <sortCondition ref="B3:B1132"/>
+  <sortState ref="A3:AT74">
+    <sortCondition ref="AQ2:AQ1130"/>
   </sortState>
   <tableColumns count="46">
     <tableColumn id="1" name="Type"/>
@@ -966,10 +966,10 @@
   <dimension ref="A1:BN1130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AN4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AR9" sqref="AR9"/>
+      <selection pane="bottomRight" activeCell="AS12" sqref="AS12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1260,12 +1260,12 @@
       <c r="BM2" s="1"/>
       <c r="BN2" s="1"/>
     </row>
-    <row r="3" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
@@ -1388,13 +1388,13 @@
         <v>0</v>
       </c>
       <c r="AQ3" s="7">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="AR3" s="7"/>
       <c r="AS3" s="7">
-        <v>1.6203703703703682E-4</v>
-      </c>
-      <c r="AT3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT3" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU3" s="1"/>
@@ -1414,7 +1414,7 @@
       <c r="BM3" s="11"/>
       <c r="BN3" s="11"/>
     </row>
-    <row r="4" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>56</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="AQ4" s="7"/>
       <c r="AR4" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AS4" s="7">
         <v>1</v>
@@ -1568,7 +1568,7 @@
       <c r="BM4" s="1"/>
       <c r="BN4" s="1"/>
     </row>
-    <row r="5" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>56</v>
       </c>
@@ -1722,12 +1722,12 @@
       <c r="BM5" s="1"/>
       <c r="BN5" s="1"/>
     </row>
-    <row r="6" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -1850,11 +1850,11 @@
         <v>0</v>
       </c>
       <c r="AQ6" s="7">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="AR6" s="7"/>
       <c r="AS6" s="7">
-        <v>1.6041666666666669E-2</v>
+        <v>1</v>
       </c>
       <c r="AT6" s="13" t="s">
         <v>55</v>
@@ -1876,12 +1876,12 @@
       <c r="BM6" s="1"/>
       <c r="BN6" s="1"/>
     </row>
-    <row r="7" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -2004,13 +2004,13 @@
         <v>0</v>
       </c>
       <c r="AQ7" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR7" s="7"/>
       <c r="AS7" s="7">
-        <v>7.081018518518542E-2</v>
-      </c>
-      <c r="AT7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU7" s="1"/>
@@ -2030,7 +2030,7 @@
       <c r="BM7" s="1"/>
       <c r="BN7" s="1"/>
     </row>
-    <row r="8" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>56</v>
       </c>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="AQ8" s="7"/>
       <c r="AR8" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AS8" s="7">
         <v>1</v>
@@ -2184,7 +2184,7 @@
       <c r="BM8" s="1"/>
       <c r="BN8" s="1"/>
     </row>
-    <row r="9" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>56</v>
       </c>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="AQ9" s="7"/>
       <c r="AR9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS9" s="7">
         <v>1</v>
@@ -2338,7 +2338,7 @@
       <c r="BM9" s="1"/>
       <c r="BN9" s="1"/>
     </row>
-    <row r="10" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>56</v>
       </c>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AQ10" s="7"/>
       <c r="AR10" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AS10" s="7">
         <v>1</v>
@@ -2492,7 +2492,7 @@
       <c r="BM10" s="1"/>
       <c r="BN10" s="1"/>
     </row>
-    <row r="11" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>56</v>
       </c>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="AQ11" s="7"/>
       <c r="AR11" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AS11" s="7">
         <v>1</v>
@@ -2646,12 +2646,12 @@
       <c r="BM11" s="1"/>
       <c r="BN11" s="1"/>
     </row>
-    <row r="12" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -2774,11 +2774,11 @@
         <v>0</v>
       </c>
       <c r="AQ12" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AR12" s="1"/>
       <c r="AS12" s="7">
-        <v>7.0648148148147918E-2</v>
+        <v>6.805555555555555E-2</v>
       </c>
       <c r="AT12" s="7" t="s">
         <v>55</v>
@@ -2800,7 +2800,7 @@
       <c r="BM12" s="1"/>
       <c r="BN12" s="1"/>
     </row>
-    <row r="13" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>56</v>
       </c>
@@ -2954,12 +2954,12 @@
       <c r="BM13" s="1"/>
       <c r="BN13" s="1"/>
     </row>
-    <row r="14" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C14" s="8">
         <v>0</v>
@@ -3082,11 +3082,11 @@
         <v>0</v>
       </c>
       <c r="AQ14" s="7">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="AR14" s="1"/>
       <c r="AS14" s="7">
-        <v>7.1296296296296524E-3</v>
+        <v>4.3749999999999997E-2</v>
       </c>
       <c r="AT14" s="13" t="s">
         <v>55</v>
@@ -3108,12 +3108,12 @@
       <c r="BM14" s="1"/>
       <c r="BN14" s="1"/>
     </row>
-    <row r="15" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
@@ -3236,11 +3236,11 @@
         <v>0</v>
       </c>
       <c r="AQ15" s="7">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="AR15" s="1"/>
       <c r="AS15" s="7">
-        <v>7.2916666666666668E-3</v>
+        <v>4.3749999999999997E-2</v>
       </c>
       <c r="AT15" s="7" t="s">
         <v>55</v>
@@ -3261,12 +3261,12 @@
       <c r="BM15" s="1"/>
       <c r="BN15" s="1"/>
     </row>
-    <row r="16" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C16" s="8">
         <v>0</v>
@@ -3389,11 +3389,11 @@
         <v>0</v>
       </c>
       <c r="AQ16" s="7">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="AR16" s="1"/>
       <c r="AS16" s="7">
-        <v>7.2916666666666668E-3</v>
+        <v>3.5648148148148123E-2</v>
       </c>
       <c r="AT16" s="13" t="s">
         <v>55</v>
@@ -3414,12 +3414,12 @@
       <c r="BM16" s="1"/>
       <c r="BN16" s="1"/>
     </row>
-    <row r="17" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3542,11 +3542,11 @@
         <v>0</v>
       </c>
       <c r="AQ17" s="7">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="AR17" s="1"/>
       <c r="AS17" s="7">
-        <v>1.8148148148148125E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="AT17" s="13" t="s">
         <v>55</v>
@@ -3567,12 +3567,12 @@
       <c r="BM17" s="1"/>
       <c r="BN17" s="1"/>
     </row>
-    <row r="18" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
@@ -3695,11 +3695,11 @@
         <v>0</v>
       </c>
       <c r="AQ18" s="7">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="AR18" s="1"/>
       <c r="AS18" s="7">
-        <v>7.9398148148147919E-3</v>
+        <v>3.4027777777777775E-2</v>
       </c>
       <c r="AT18" s="7" t="s">
         <v>55</v>
@@ -3720,12 +3720,12 @@
       <c r="BM18" s="1"/>
       <c r="BN18" s="1"/>
     </row>
-    <row r="19" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C19" s="8">
         <v>0</v>
@@ -3848,11 +3848,11 @@
         <v>0</v>
       </c>
       <c r="AQ19" s="7">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="AR19" s="1"/>
       <c r="AS19" s="7">
-        <v>9.7222222222222224E-3</v>
+        <v>3.111111111111111E-2</v>
       </c>
       <c r="AT19" s="7" t="s">
         <v>55</v>
@@ -3873,12 +3873,12 @@
       <c r="BM19" s="1"/>
       <c r="BN19" s="1"/>
     </row>
-    <row r="20" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>
@@ -4001,13 +4001,13 @@
         <v>0</v>
       </c>
       <c r="AQ20" s="7">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AR20" s="1"/>
       <c r="AS20" s="7">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="AT20" s="7" t="s">
+        <v>2.9814814814814794E-2</v>
+      </c>
+      <c r="AT20" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU20" s="1"/>
@@ -4026,12 +4026,12 @@
       <c r="BM20" s="1"/>
       <c r="BN20" s="1"/>
     </row>
-    <row r="21" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>
@@ -4154,13 +4154,13 @@
         <v>0</v>
       </c>
       <c r="AQ21" s="7">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="AR21" s="1"/>
       <c r="AS21" s="7">
-        <v>9.7222222222222224E-3</v>
-      </c>
-      <c r="AT21" s="7" t="s">
+        <v>2.9004629629629654E-2</v>
+      </c>
+      <c r="AT21" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU21" s="1"/>
@@ -4179,12 +4179,12 @@
       <c r="BM21" s="1"/>
       <c r="BN21" s="1"/>
     </row>
-    <row r="22" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C22" s="8">
         <v>0</v>
@@ -4307,13 +4307,13 @@
         <v>0</v>
       </c>
       <c r="AQ22" s="7">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="AR22" s="1"/>
       <c r="AS22" s="7">
-        <v>1.6203703703703682E-4</v>
-      </c>
-      <c r="AT22" s="7" t="s">
+        <v>2.8356481481481458E-2</v>
+      </c>
+      <c r="AT22" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU22" s="1"/>
@@ -4332,7 +4332,7 @@
       <c r="BM22" s="1"/>
       <c r="BN22" s="1"/>
     </row>
-    <row r="23" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>56</v>
       </c>
@@ -4485,12 +4485,12 @@
       <c r="BM23" s="1"/>
       <c r="BN23" s="1"/>
     </row>
-    <row r="24" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="C24" s="8">
         <v>0</v>
@@ -4613,13 +4613,13 @@
         <v>0</v>
       </c>
       <c r="AQ24" s="7">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="AR24" s="1"/>
       <c r="AS24" s="7">
-        <v>4.861111111111111E-4</v>
-      </c>
-      <c r="AT24" s="13" t="s">
+        <v>2.4467592592592569E-2</v>
+      </c>
+      <c r="AT24" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU24" s="1"/>
@@ -4638,12 +4638,12 @@
       <c r="BM24" s="1"/>
       <c r="BN24" s="1"/>
     </row>
-    <row r="25" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="C25" s="8">
         <v>0</v>
@@ -4766,13 +4766,13 @@
         <v>0</v>
       </c>
       <c r="AQ25" s="7">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="AR25" s="1"/>
       <c r="AS25" s="7">
-        <v>3.2407407407407434E-4</v>
-      </c>
-      <c r="AT25" s="13" t="s">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="AT25" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU25" s="1"/>
@@ -4791,12 +4791,12 @@
       <c r="BM25" s="1"/>
       <c r="BN25" s="1"/>
     </row>
-    <row r="26" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C26" s="8">
         <v>0</v>
@@ -4919,13 +4919,13 @@
         <v>0</v>
       </c>
       <c r="AQ26" s="7">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="AR26" s="1"/>
       <c r="AS26" s="7">
-        <v>8.1018518518518755E-4</v>
-      </c>
-      <c r="AT26" s="7" t="s">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="AT26" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU26" s="1"/>
@@ -4944,12 +4944,12 @@
       <c r="BM26" s="1"/>
       <c r="BN26" s="1"/>
     </row>
-    <row r="27" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C27" s="8">
         <v>0</v>
@@ -5072,11 +5072,11 @@
         <v>0</v>
       </c>
       <c r="AQ27" s="7">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="AR27" s="1"/>
       <c r="AS27" s="7">
-        <v>8.1018518518518755E-4</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="AT27" s="13" t="s">
         <v>55</v>
@@ -5097,12 +5097,12 @@
       <c r="BM27" s="1"/>
       <c r="BN27" s="1"/>
     </row>
-    <row r="28" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C28" s="8">
         <v>0</v>
@@ -5225,13 +5225,13 @@
         <v>0</v>
       </c>
       <c r="AQ28" s="7">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="AR28" s="1"/>
       <c r="AS28" s="7">
-        <v>1.6203703703703682E-4</v>
-      </c>
-      <c r="AT28" s="7" t="s">
+        <v>2.3981481481481461E-2</v>
+      </c>
+      <c r="AT28" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU28" s="1"/>
@@ -5250,12 +5250,12 @@
       <c r="BM28" s="1"/>
       <c r="BN28" s="1"/>
     </row>
-    <row r="29" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C29" s="8">
         <v>0</v>
@@ -5378,11 +5378,11 @@
         <v>0</v>
       </c>
       <c r="AQ29" s="7">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="AR29" s="1"/>
       <c r="AS29" s="7">
-        <v>1.6203703703703682E-4</v>
+        <v>1.8148148148148125E-2</v>
       </c>
       <c r="AT29" s="13" t="s">
         <v>55</v>
@@ -5403,7 +5403,7 @@
       <c r="BM29" s="1"/>
       <c r="BN29" s="1"/>
     </row>
-    <row r="30" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>56</v>
       </c>
@@ -5556,12 +5556,12 @@
       <c r="BM30" s="1"/>
       <c r="BN30" s="1"/>
     </row>
-    <row r="31" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C31" s="8">
         <v>0</v>
@@ -5684,13 +5684,13 @@
         <v>0</v>
       </c>
       <c r="AQ31" s="7">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="AR31" s="1"/>
       <c r="AS31" s="7">
-        <v>1.6203703703703682E-4</v>
-      </c>
-      <c r="AT31" s="7" t="s">
+        <v>1.6041666666666669E-2</v>
+      </c>
+      <c r="AT31" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU31" s="1"/>
@@ -5709,12 +5709,12 @@
       <c r="BM31" s="1"/>
       <c r="BN31" s="1"/>
     </row>
-    <row r="32" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C32" s="8">
         <v>0</v>
@@ -5837,13 +5837,13 @@
         <v>0</v>
       </c>
       <c r="AQ32" s="7">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="AR32" s="1"/>
       <c r="AS32" s="7">
-        <v>3.4027777777777775E-2</v>
-      </c>
-      <c r="AT32" s="7" t="s">
+        <v>1.4583333333333334E-2</v>
+      </c>
+      <c r="AT32" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU32" s="1"/>
@@ -5862,12 +5862,12 @@
       <c r="BM32" s="1"/>
       <c r="BN32" s="1"/>
     </row>
-    <row r="33" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="C33" s="8">
         <v>0</v>
@@ -5990,13 +5990,13 @@
         <v>0</v>
       </c>
       <c r="AQ33" s="7">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AR33" s="1"/>
       <c r="AS33" s="7">
-        <v>2.8356481481481458E-2</v>
-      </c>
-      <c r="AT33" s="13" t="s">
+        <v>1.0532407407407431E-2</v>
+      </c>
+      <c r="AT33" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU33" s="1"/>
@@ -6015,12 +6015,12 @@
       <c r="BM33" s="1"/>
       <c r="BN33" s="1"/>
     </row>
-    <row r="34" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="C34" s="8">
         <v>0</v>
@@ -6143,11 +6143,11 @@
         <v>0</v>
       </c>
       <c r="AQ34" s="7">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="AR34" s="1"/>
       <c r="AS34" s="7">
-        <v>2.4467592592592569E-2</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="AT34" s="7" t="s">
         <v>55</v>
@@ -6168,12 +6168,12 @@
       <c r="BM34" s="1"/>
       <c r="BN34" s="1"/>
     </row>
-    <row r="35" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C35" s="8">
         <v>0</v>
@@ -6296,13 +6296,13 @@
         <v>0</v>
       </c>
       <c r="AQ35" s="7">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="AR35" s="1"/>
       <c r="AS35" s="7">
-        <v>1.6203703703703682E-4</v>
-      </c>
-      <c r="AT35" s="13" t="s">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="AT35" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU35" s="1"/>
@@ -6321,7 +6321,7 @@
       <c r="BM35" s="1"/>
       <c r="BN35" s="1"/>
     </row>
-    <row r="36" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>56</v>
       </c>
@@ -6474,12 +6474,12 @@
       <c r="BM36" s="1"/>
       <c r="BN36" s="1"/>
     </row>
-    <row r="37" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C37" s="8">
         <v>0</v>
@@ -6602,13 +6602,13 @@
         <v>0</v>
       </c>
       <c r="AQ37" s="7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AR37" s="1"/>
       <c r="AS37" s="7">
-        <v>1.4583333333333334E-2</v>
-      </c>
-      <c r="AT37" s="13" t="s">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="AT37" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU37" s="1"/>
@@ -6627,12 +6627,12 @@
       <c r="BM37" s="1"/>
       <c r="BN37" s="1"/>
     </row>
-    <row r="38" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C38" s="8">
         <v>0</v>
@@ -6755,11 +6755,11 @@
         <v>0</v>
       </c>
       <c r="AQ38" s="7">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="AR38" s="1"/>
       <c r="AS38" s="7">
-        <v>3.2407407407407434E-4</v>
+        <v>8.4259259259259027E-3</v>
       </c>
       <c r="AT38" s="7" t="s">
         <v>55</v>
@@ -6780,12 +6780,12 @@
       <c r="BM38" s="1"/>
       <c r="BN38" s="1"/>
     </row>
-    <row r="39" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="C39" s="8">
         <v>0</v>
@@ -6908,13 +6908,13 @@
         <v>0</v>
       </c>
       <c r="AQ39" s="7">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="AR39" s="1"/>
       <c r="AS39" s="7">
-        <v>2.9814814814814794E-2</v>
-      </c>
-      <c r="AT39" s="13" t="s">
+        <v>8.4259259259259027E-3</v>
+      </c>
+      <c r="AT39" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU39" s="1"/>
@@ -6933,12 +6933,12 @@
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
     </row>
-    <row r="40" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="C40" s="8">
         <v>0</v>
@@ -7061,11 +7061,11 @@
         <v>0</v>
       </c>
       <c r="AQ40" s="7">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="AR40" s="1"/>
       <c r="AS40" s="7">
-        <v>6.805555555555555E-2</v>
+        <v>7.9398148148147919E-3</v>
       </c>
       <c r="AT40" s="7" t="s">
         <v>55</v>
@@ -7086,7 +7086,7 @@
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
     </row>
-    <row r="41" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>56</v>
       </c>
@@ -7215,7 +7215,7 @@
       </c>
       <c r="AQ41" s="7"/>
       <c r="AR41" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AS41" s="7">
         <v>1</v>
@@ -7239,12 +7239,12 @@
       <c r="BM41" s="1"/>
       <c r="BN41" s="1"/>
     </row>
-    <row r="42" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C42" s="8">
         <v>0</v>
@@ -7367,13 +7367,13 @@
         <v>0</v>
       </c>
       <c r="AQ42" s="7">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="AR42" s="1"/>
       <c r="AS42" s="7">
-        <v>1.4583333333333334E-3</v>
-      </c>
-      <c r="AT42" s="7" t="s">
+        <v>7.2916666666666668E-3</v>
+      </c>
+      <c r="AT42" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU42" s="1"/>
@@ -7392,12 +7392,12 @@
       <c r="BM42" s="1"/>
       <c r="BN42" s="1"/>
     </row>
-    <row r="43" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C43" s="8">
         <v>0</v>
@@ -7520,13 +7520,13 @@
         <v>0</v>
       </c>
       <c r="AQ43" s="7">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="AR43" s="1"/>
       <c r="AS43" s="7">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="AT43" s="13" t="s">
+        <v>7.2916666666666668E-3</v>
+      </c>
+      <c r="AT43" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU43" s="1"/>
@@ -7545,12 +7545,12 @@
       <c r="BM43" s="1"/>
       <c r="BN43" s="1"/>
     </row>
-    <row r="44" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C44" s="8">
         <v>0</v>
@@ -7673,11 +7673,11 @@
         <v>0</v>
       </c>
       <c r="AQ44" s="7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AR44" s="1"/>
       <c r="AS44" s="7">
-        <v>1.2962962962962986E-3</v>
+        <v>7.1296296296296524E-3</v>
       </c>
       <c r="AT44" s="13" t="s">
         <v>55</v>
@@ -7698,12 +7698,12 @@
       <c r="BM44" s="1"/>
       <c r="BN44" s="1"/>
     </row>
-    <row r="45" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="C45" s="8">
         <v>0</v>
@@ -7826,11 +7826,11 @@
         <v>0</v>
       </c>
       <c r="AQ45" s="7">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AR45" s="1"/>
       <c r="AS45" s="7">
-        <v>1.0532407407407431E-2</v>
+        <v>6.4814814814814796E-3</v>
       </c>
       <c r="AT45" s="7" t="s">
         <v>55</v>
@@ -7851,7 +7851,7 @@
       <c r="BM45" s="1"/>
       <c r="BN45" s="1"/>
     </row>
-    <row r="46" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>56</v>
       </c>
@@ -8004,12 +8004,12 @@
       <c r="BM46" s="1"/>
       <c r="BN46" s="1"/>
     </row>
-    <row r="47" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C47" s="8">
         <v>0</v>
@@ -8132,11 +8132,11 @@
         <v>0</v>
       </c>
       <c r="AQ47" s="7">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="AR47" s="1"/>
       <c r="AS47" s="7">
-        <v>4.3749999999999997E-2</v>
+        <v>6.4814814814814796E-3</v>
       </c>
       <c r="AT47" s="7" t="s">
         <v>55</v>
@@ -8157,12 +8157,12 @@
       <c r="BM47" s="1"/>
       <c r="BN47" s="1"/>
     </row>
-    <row r="48" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C48" s="8">
         <v>0</v>
@@ -8285,13 +8285,13 @@
         <v>0</v>
       </c>
       <c r="AQ48" s="7">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="AR48" s="1"/>
       <c r="AS48" s="7">
-        <v>8.4259259259259027E-3</v>
-      </c>
-      <c r="AT48" s="7" t="s">
+        <v>6.4814814814814796E-3</v>
+      </c>
+      <c r="AT48" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU48" s="1"/>
@@ -8310,12 +8310,12 @@
       <c r="BM48" s="1"/>
       <c r="BN48" s="1"/>
     </row>
-    <row r="49" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C49" s="8">
         <v>0</v>
@@ -8438,13 +8438,13 @@
         <v>0</v>
       </c>
       <c r="AQ49" s="7">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="AR49" s="1"/>
       <c r="AS49" s="7">
-        <v>8.4259259259259027E-3</v>
-      </c>
-      <c r="AT49" s="7" t="s">
+        <v>2.5925925925925903E-3</v>
+      </c>
+      <c r="AT49" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU49" s="1"/>
@@ -8463,12 +8463,12 @@
       <c r="BM49" s="1"/>
       <c r="BN49" s="1"/>
     </row>
-    <row r="50" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C50" s="8">
         <v>0</v>
@@ -8591,11 +8591,11 @@
         <v>0</v>
       </c>
       <c r="AQ50" s="7">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="AR50" s="1"/>
       <c r="AS50" s="7">
-        <v>2.4305555555555556E-2</v>
+        <v>1.6203703703703679E-3</v>
       </c>
       <c r="AT50" s="13" t="s">
         <v>55</v>
@@ -8616,12 +8616,12 @@
       <c r="BM50" s="1"/>
       <c r="BN50" s="1"/>
     </row>
-    <row r="51" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C51" s="8">
         <v>0</v>
@@ -8744,11 +8744,11 @@
         <v>0</v>
       </c>
       <c r="AQ51" s="7">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="AR51" s="1"/>
       <c r="AS51" s="7">
-        <v>4.3749999999999997E-2</v>
+        <v>1.6203703703703679E-3</v>
       </c>
       <c r="AT51" s="13" t="s">
         <v>55</v>
@@ -8769,12 +8769,12 @@
       <c r="BM51" s="1"/>
       <c r="BN51" s="1"/>
     </row>
-    <row r="52" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>140</v>
+      <c r="B52" s="15" t="s">
+        <v>77</v>
       </c>
       <c r="C52" s="8">
         <v>0</v>
@@ -8897,11 +8897,11 @@
         <v>0</v>
       </c>
       <c r="AQ52" s="7">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="AR52" s="1"/>
       <c r="AS52" s="7">
-        <v>1</v>
+        <v>1.6203703703703679E-3</v>
       </c>
       <c r="AT52" s="7" t="s">
         <v>55</v>
@@ -8922,12 +8922,12 @@
       <c r="BM52" s="1"/>
       <c r="BN52" s="1"/>
     </row>
-    <row r="53" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C53" s="8">
         <v>0</v>
@@ -9050,13 +9050,13 @@
         <v>0</v>
       </c>
       <c r="AQ53" s="7">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="AR53" s="1"/>
       <c r="AS53" s="7">
-        <v>2.9004629629629654E-2</v>
-      </c>
-      <c r="AT53" s="13" t="s">
+        <v>1.4583333333333334E-3</v>
+      </c>
+      <c r="AT53" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU53" s="1"/>
@@ -9075,12 +9075,12 @@
       <c r="BM53" s="1"/>
       <c r="BN53" s="1"/>
     </row>
-    <row r="54" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C54" s="8">
         <v>0</v>
@@ -9203,11 +9203,11 @@
         <v>0</v>
       </c>
       <c r="AQ54" s="7">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AR54" s="1"/>
       <c r="AS54" s="7">
-        <v>1.6203703703703679E-3</v>
+        <v>1.2962962962962986E-3</v>
       </c>
       <c r="AT54" s="13" t="s">
         <v>55</v>
@@ -9228,7 +9228,7 @@
       <c r="BM54" s="1"/>
       <c r="BN54" s="1"/>
     </row>
-    <row r="55" spans="1:66" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:66" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>56</v>
       </c>
@@ -9357,7 +9357,7 @@
       </c>
       <c r="AQ55" s="7"/>
       <c r="AR55" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AS55" s="7">
         <v>1</v>
@@ -9382,7 +9382,7 @@
       <c r="BM55" s="1"/>
       <c r="BN55" s="1"/>
     </row>
-    <row r="56" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
         <v>56</v>
       </c>
@@ -9511,7 +9511,7 @@
       </c>
       <c r="AQ56" s="1"/>
       <c r="AR56" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AS56" s="7">
         <v>1</v>
@@ -9536,7 +9536,7 @@
       <c r="BM56" s="1"/>
       <c r="BN56" s="1"/>
     </row>
-    <row r="57" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>56</v>
       </c>
@@ -9690,7 +9690,7 @@
       <c r="BM57" s="7"/>
       <c r="BN57" s="7"/>
     </row>
-    <row r="58" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -9844,7 +9844,7 @@
       <c r="BM58" s="1"/>
       <c r="BN58" s="1"/>
     </row>
-    <row r="59" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>56</v>
       </c>
@@ -9998,12 +9998,12 @@
       <c r="BM59" s="1"/>
       <c r="BN59" s="1"/>
     </row>
-    <row r="60" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C60" s="8">
         <v>0</v>
@@ -10126,13 +10126,13 @@
         <v>0</v>
       </c>
       <c r="AQ60" s="1">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="AR60" s="7"/>
       <c r="AS60" s="7">
-        <v>9.7384259259259032E-2</v>
-      </c>
-      <c r="AT60" s="7" t="s">
+        <v>1.2962962962962986E-3</v>
+      </c>
+      <c r="AT60" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU60" s="1"/>
@@ -10152,12 +10152,12 @@
       <c r="BM60" s="1"/>
       <c r="BN60" s="1"/>
     </row>
-    <row r="61" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C61" s="8">
         <v>0</v>
@@ -10280,11 +10280,11 @@
         <v>0</v>
       </c>
       <c r="AQ61" s="1">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="AR61" s="7"/>
       <c r="AS61" s="7">
-        <v>2.4305555555555556E-2</v>
+        <v>8.1018518518518755E-4</v>
       </c>
       <c r="AT61" s="13" t="s">
         <v>55</v>
@@ -10306,12 +10306,12 @@
       <c r="BM61" s="1"/>
       <c r="BN61" s="1"/>
     </row>
-    <row r="62" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C62" s="8">
         <v>0</v>
@@ -10434,13 +10434,13 @@
         <v>0</v>
       </c>
       <c r="AQ62" s="1">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="AR62" s="7"/>
       <c r="AS62" s="7">
-        <v>2.3981481481481461E-2</v>
-      </c>
-      <c r="AT62" s="13" t="s">
+        <v>8.1018518518518755E-4</v>
+      </c>
+      <c r="AT62" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU62" s="1"/>
@@ -10460,12 +10460,12 @@
       <c r="BM62" s="1"/>
       <c r="BN62" s="1"/>
     </row>
-    <row r="63" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="C63" s="8">
         <v>0</v>
@@ -10588,11 +10588,11 @@
         <v>0</v>
       </c>
       <c r="AQ63" s="1">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="AR63" s="7"/>
       <c r="AS63" s="7">
-        <v>9.7222222222222224E-3</v>
+        <v>6.4814814814814791E-4</v>
       </c>
       <c r="AT63" s="7" t="s">
         <v>55</v>
@@ -10614,12 +10614,12 @@
       <c r="BM63" s="1"/>
       <c r="BN63" s="1"/>
     </row>
-    <row r="64" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="C64" s="8">
         <v>0</v>
@@ -10742,11 +10742,11 @@
         <v>0</v>
       </c>
       <c r="AQ64" s="1">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="AR64" s="7"/>
       <c r="AS64" s="7">
-        <v>1.2962962962962986E-3</v>
+        <v>4.861111111111111E-4</v>
       </c>
       <c r="AT64" s="13" t="s">
         <v>55</v>
@@ -10768,12 +10768,12 @@
       <c r="BM64" s="1"/>
       <c r="BN64" s="1"/>
     </row>
-    <row r="65" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="C65" s="8">
         <v>0</v>
@@ -10896,13 +10896,13 @@
         <v>0</v>
       </c>
       <c r="AQ65" s="1">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="AR65" s="7"/>
       <c r="AS65" s="7">
-        <v>3.5648148148148123E-2</v>
-      </c>
-      <c r="AT65" s="13" t="s">
+        <v>3.2407407407407434E-4</v>
+      </c>
+      <c r="AT65" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU65" s="1"/>
@@ -10922,7 +10922,7 @@
       <c r="BM65" s="1"/>
       <c r="BN65" s="1"/>
     </row>
-    <row r="66" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>56</v>
       </c>
@@ -11051,7 +11051,7 @@
       </c>
       <c r="AQ66" s="1"/>
       <c r="AR66" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AS66" s="7">
         <v>1</v>
@@ -11076,12 +11076,12 @@
       <c r="BM66" s="1"/>
       <c r="BN66" s="1"/>
     </row>
-    <row r="67" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="C67" s="8">
         <v>0</v>
@@ -11204,13 +11204,13 @@
         <v>0</v>
       </c>
       <c r="AQ67" s="1">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="AR67" s="7"/>
       <c r="AS67" s="7">
-        <v>3.111111111111111E-2</v>
-      </c>
-      <c r="AT67" s="7" t="s">
+        <v>3.2407407407407434E-4</v>
+      </c>
+      <c r="AT67" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU67" s="1"/>
@@ -11230,12 +11230,12 @@
       <c r="BM67" s="1"/>
       <c r="BN67" s="1"/>
     </row>
-    <row r="68" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="C68" s="8">
         <v>0</v>
@@ -11358,13 +11358,13 @@
         <v>0</v>
       </c>
       <c r="AQ68" s="1">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="AR68" s="7"/>
       <c r="AS68" s="7">
-        <v>6.4814814814814791E-4</v>
-      </c>
-      <c r="AT68" s="7" t="s">
+        <v>1.6203703703703682E-4</v>
+      </c>
+      <c r="AT68" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU68" s="1"/>
@@ -11384,12 +11384,12 @@
       <c r="BM68" s="1"/>
       <c r="BN68" s="1"/>
     </row>
-    <row r="69" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C69" s="8">
         <v>0</v>
@@ -11512,13 +11512,13 @@
         <v>0</v>
       </c>
       <c r="AQ69" s="1">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="AR69" s="7"/>
       <c r="AS69" s="7">
-        <v>2.5925925925925903E-3</v>
-      </c>
-      <c r="AT69" s="13" t="s">
+        <v>1.6203703703703682E-4</v>
+      </c>
+      <c r="AT69" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU69" s="1"/>
@@ -11540,12 +11540,12 @@
       <c r="BM69" s="1"/>
       <c r="BN69" s="1"/>
     </row>
-    <row r="70" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C70" s="8">
         <v>0</v>
@@ -11668,11 +11668,11 @@
         <v>0</v>
       </c>
       <c r="AQ70" s="1">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="AR70" s="7"/>
       <c r="AS70" s="7">
-        <v>6.4814814814814796E-3</v>
+        <v>1.6203703703703682E-4</v>
       </c>
       <c r="AT70" s="7" t="s">
         <v>55</v>
@@ -11696,12 +11696,12 @@
       <c r="BM70" s="1"/>
       <c r="BN70" s="1"/>
     </row>
-    <row r="71" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C71" s="8">
         <v>0</v>
@@ -11824,13 +11824,13 @@
         <v>0</v>
       </c>
       <c r="AQ71" s="1">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="AR71" s="7"/>
       <c r="AS71" s="7">
-        <v>1.6203703703703679E-3</v>
-      </c>
-      <c r="AT71" s="7" t="s">
+        <v>1.6203703703703682E-4</v>
+      </c>
+      <c r="AT71" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU71" s="1"/>
@@ -11852,12 +11852,12 @@
       <c r="BM71" s="1"/>
       <c r="BN71" s="1"/>
     </row>
-    <row r="72" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="C72" s="8">
         <v>0</v>
@@ -11980,13 +11980,13 @@
         <v>0</v>
       </c>
       <c r="AQ72" s="1">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="AR72" s="7"/>
       <c r="AS72" s="7">
-        <v>1.6203703703703679E-3</v>
-      </c>
-      <c r="AT72" s="13" t="s">
+        <v>1.6203703703703682E-4</v>
+      </c>
+      <c r="AT72" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU72" s="1"/>
@@ -12008,12 +12008,12 @@
       <c r="BM72" s="1"/>
       <c r="BN72" s="1"/>
     </row>
-    <row r="73" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="C73" s="8">
         <v>0</v>
@@ -12136,13 +12136,13 @@
         <v>0</v>
       </c>
       <c r="AQ73" s="1">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="AR73" s="7"/>
       <c r="AS73" s="7">
-        <v>6.4814814814814796E-3</v>
-      </c>
-      <c r="AT73" s="7" t="s">
+        <v>1.6203703703703682E-4</v>
+      </c>
+      <c r="AT73" s="13" t="s">
         <v>55</v>
       </c>
       <c r="AU73" s="1"/>
@@ -12164,12 +12164,12 @@
       <c r="BM73" s="1"/>
       <c r="BN73" s="1"/>
     </row>
-    <row r="74" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B74" s="15" t="s">
-        <v>74</v>
+      <c r="B74" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="C74" s="8">
         <v>0</v>
@@ -12292,13 +12292,13 @@
         <v>0</v>
       </c>
       <c r="AQ74" s="1">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="AR74" s="7"/>
       <c r="AS74" s="7">
-        <v>6.4814814814814796E-3</v>
-      </c>
-      <c r="AT74" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT74" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AU74" s="1"/>
@@ -12320,7 +12320,7 @@
       <c r="BM74" s="1"/>
       <c r="BN74" s="1"/>
     </row>
-    <row r="75" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>56</v>
       </c>
@@ -12476,7 +12476,7 @@
       <c r="BM75" s="1"/>
       <c r="BN75" s="1"/>
     </row>
-    <row r="76" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>56</v>
       </c>
@@ -12632,7 +12632,7 @@
       <c r="BM76" s="1"/>
       <c r="BN76" s="1"/>
     </row>
-    <row r="77" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>56</v>
       </c>
@@ -12788,7 +12788,7 @@
       <c r="BM77" s="1"/>
       <c r="BN77" s="1"/>
     </row>
-    <row r="78" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>56</v>
       </c>
@@ -12944,7 +12944,7 @@
       <c r="BM78" s="1"/>
       <c r="BN78" s="1"/>
     </row>
-    <row r="79" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>56</v>
       </c>
@@ -13073,7 +13073,7 @@
       </c>
       <c r="AQ79" s="1"/>
       <c r="AR79" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AS79" s="7">
         <v>1</v>
@@ -13100,7 +13100,7 @@
       <c r="BM79" s="1"/>
       <c r="BN79" s="1"/>
     </row>
-    <row r="80" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>56</v>
       </c>
@@ -13256,7 +13256,7 @@
       <c r="BM80" s="1"/>
       <c r="BN80" s="1"/>
     </row>
-    <row r="81" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>56</v>
       </c>
@@ -13412,7 +13412,7 @@
       <c r="BM81" s="1"/>
       <c r="BN81" s="1"/>
     </row>
-    <row r="82" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>56</v>
       </c>
@@ -13568,7 +13568,7 @@
       <c r="BM82" s="1"/>
       <c r="BN82" s="1"/>
     </row>
-    <row r="83" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>56</v>
       </c>
@@ -13724,7 +13724,7 @@
       <c r="BM83" s="1"/>
       <c r="BN83" s="1"/>
     </row>
-    <row r="84" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>56</v>
       </c>
@@ -13853,7 +13853,7 @@
       </c>
       <c r="AQ84" s="1"/>
       <c r="AR84" s="7">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="AS84" s="7">
         <v>1</v>
@@ -13880,7 +13880,7 @@
       <c r="BM84" s="1"/>
       <c r="BN84" s="1"/>
     </row>
-    <row r="85" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>56</v>
       </c>
@@ -14009,7 +14009,7 @@
       </c>
       <c r="AQ85" s="1"/>
       <c r="AR85" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AS85" s="7">
         <v>1</v>
@@ -14036,7 +14036,7 @@
       <c r="BM85" s="1"/>
       <c r="BN85" s="1"/>
     </row>
-    <row r="86" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:66" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>56</v>
       </c>
@@ -14165,7 +14165,7 @@
       </c>
       <c r="AQ86" s="7"/>
       <c r="AR86" s="7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AS86" s="7">
         <v>1</v>

</xml_diff>